<commit_message>
pulled data using 1% detection
</commit_message>
<xml_diff>
--- a/core_microbiome/core_microbiome_species.xlsx
+++ b/core_microbiome/core_microbiome_species.xlsx
@@ -5,17 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alicia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alicia/Desktop/MICB-475-Team-2/core_microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C28287A-BEFD-994E-9D6F-233D703A754D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013C482A-BC78-D344-B388-4953E753D7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9BCC909C-BB86-064A-9F21-5D155E6D1246}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{9BCC909C-BB86-064A-9F21-5D155E6D1246}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2%" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="1%" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1%'!$A$2:$H$7</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="56">
   <si>
     <t>Domain</t>
   </si>
@@ -123,6 +128,87 @@
   </si>
   <si>
     <t>untreated ASVs</t>
+  </si>
+  <si>
+    <t>eb1cb381c314ecbbf46265b2e2351ee8</t>
+  </si>
+  <si>
+    <t>4a21bd45b5ff48f40bbcadf6930fc3ee</t>
+  </si>
+  <si>
+    <t>o__Lachnospirales</t>
+  </si>
+  <si>
+    <t>f__Lachnospiraceae</t>
+  </si>
+  <si>
+    <t>g__Agathobacter</t>
+  </si>
+  <si>
+    <t>3d846e34d0ebbaa6096f5b1e5e8afa03</t>
+  </si>
+  <si>
+    <t>f__Oscillospiraceae</t>
+  </si>
+  <si>
+    <t>g__UCG-002</t>
+  </si>
+  <si>
+    <t>s__uncultured_organism</t>
+  </si>
+  <si>
+    <t>22436f090b3327aa9cc25a46c2614ab0</t>
+  </si>
+  <si>
+    <t>43c6b4b7d67b71ca2cba59db1b71e4ef</t>
+  </si>
+  <si>
+    <t>c560a89bbad32dad461cf90eda5e1c97</t>
+  </si>
+  <si>
+    <t>g__Subdoligranulum</t>
+  </si>
+  <si>
+    <t>0bc4e35da130d9cb9fc1090c80011153</t>
+  </si>
+  <si>
+    <t>f__Rikenellaceae</t>
+  </si>
+  <si>
+    <t>g__Alistipes</t>
+  </si>
+  <si>
+    <t>fbbeae3dceada6928b2cdc472f5d9901</t>
+  </si>
+  <si>
+    <t>p__Verrucomicrobiota</t>
+  </si>
+  <si>
+    <t>c__Verrucomicrobiae</t>
+  </si>
+  <si>
+    <t>o__Verrucomicrobiales</t>
+  </si>
+  <si>
+    <t>f__Akkermansiaceae</t>
+  </si>
+  <si>
+    <t>g__Akkermansia</t>
+  </si>
+  <si>
+    <t>s__Akkermansia_muciniphila</t>
+  </si>
+  <si>
+    <t>76aa915543cd876d620ebeafeb9fd767</t>
+  </si>
+  <si>
+    <t>f__Tannerellaceae</t>
+  </si>
+  <si>
+    <t>g__Parabacteroides</t>
+  </si>
+  <si>
+    <t>s__Parabacteroides_merdae</t>
   </si>
 </sst>
 </file>
@@ -198,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -214,11 +300,303 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -531,7 +909,7 @@
   <dimension ref="A2:H26"/>
   <sheetViews>
     <sheetView zoomScale="136" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -923,6 +1301,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="d71fe">
+      <formula>NOT(ISERROR(SEARCH("d71fe",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="96c7c">
+      <formula>NOT(ISERROR(SEARCH("96c7c",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="76d6b">
+      <formula>NOT(ISERROR(SEARCH("76d6b",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -932,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200C248-5114-194D-9FD4-1D78E0AB01F2}">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="139" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1273,6 +1662,1882 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="76d6b">
+      <formula>NOT(ISERROR(SEARCH("76d6b",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93598962-E610-874D-AD56-358811F697AD}">
+  <dimension ref="A2:H45"/>
+  <sheetViews>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="d71fe67e73a45e78b36ab2586bb5dcc8">
+      <formula>NOT(ISERROR(SEARCH("d71fe67e73a45e78b36ab2586bb5dcc8",A4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="d71">
+      <formula>NOT(ISERROR(SEARCH("d71",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="96c">
+      <formula>NOT(ISERROR(SEARCH("96c",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="eb1">
+      <formula>NOT(ISERROR(SEARCH("eb1",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="76d6b">
+      <formula>NOT(ISERROR(SEARCH("76d6b",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10510B0A-CE68-1642-8031-F5A089ABAC3E}">
+  <dimension ref="A2:H45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="d71">
+      <formula>NOT(ISERROR(SEARCH("d71",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="96c">
+      <formula>NOT(ISERROR(SEARCH("96c",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="76d6b">
+      <formula>NOT(ISERROR(SEARCH("76d6b",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>